<commit_message>
More link budget tweaks
</commit_message>
<xml_diff>
--- a/Ground Station/Sprite Link Budget.xlsx
+++ b/Ground Station/Sprite Link Budget.xlsx
@@ -4,19 +4,18 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="22416"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14760"/>
+    <workbookView xWindow="2880" yWindow="1040" windowWidth="25600" windowHeight="14760"/>
   </bookViews>
   <sheets>
     <sheet name="Link Budget" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">'Link Budget'!$A$1:$I$55</definedName>
   </definedNames>
   <calcPr calcId="140001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="P - Personal View" guid="{56B56577-359B-4FEF-8511-5634C3B3AD8C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1017" windowHeight="629" activeSheetId="1"/>
     <customWorkbookView name="Justin Atchison - Personal View" guid="{DF438D20-ED32-4502-BBF3-1338727B4A2A}" mergeInterval="0" personalView="1" maximized="1" xWindow="1" yWindow="1" windowWidth="1011" windowHeight="646" activeSheetId="1"/>
-    <customWorkbookView name="P - Personal View" guid="{56B56577-359B-4FEF-8511-5634C3B3AD8C}" mergeInterval="0" personalView="1" maximized="1" windowWidth="1017" windowHeight="629" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -27,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="78">
   <si>
     <t>Boltzmann Constant, k</t>
   </si>
@@ -254,70 +253,7 @@
     <t>*Boxes with black outlines are inputs</t>
   </si>
   <si>
-    <t>Sprite2 Chip Spacecraft</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>T = 2*pi*sqrt((RE+h)^3/mu)</t>
-  </si>
-  <si>
-    <t>Time Overhead, t</t>
-  </si>
-  <si>
-    <t>t = T/180*(asin((S/(RE+h))*sin(90-φ))</t>
-  </si>
-  <si>
-    <t>v = sqrt(mu/(RE+h))</t>
-  </si>
-  <si>
-    <t>vr = v*cos(elevation)</t>
-  </si>
-  <si>
-    <t>|df| = vr*f/c</t>
-  </si>
-  <si>
-    <t>Ls = (λ / 4πS)^2</t>
-  </si>
-  <si>
-    <t>Noise Temperature at Antenna, T</t>
-  </si>
-  <si>
     <t>Receiver Noise Factor/Figure</t>
-  </si>
-  <si>
-    <t>B &gt; 2*Rc</t>
-  </si>
-  <si>
-    <t>System Noise Power, N</t>
-  </si>
-  <si>
-    <t>N = k Ts B</t>
-  </si>
-  <si>
-    <t>Line Losses etc.</t>
-  </si>
-  <si>
-    <t>Length of Signal, ts</t>
-  </si>
-  <si>
-    <t>s</t>
-  </si>
-  <si>
-    <t>Number of Bits Transmitted</t>
-  </si>
-  <si>
-    <t>Gsp = Rc/R</t>
-  </si>
-  <si>
-    <t>Received Power,  C</t>
-  </si>
-  <si>
-    <t>C = Pt+La+Ls+Lp+Gr+Gt-M</t>
-  </si>
-  <si>
-    <t>S = C+Gsp</t>
   </si>
   <si>
     <t>&lt;- Receiver system noise temperature goes here</t>
@@ -337,7 +273,7 @@
     <numFmt numFmtId="167" formatCode="0.0000"/>
     <numFmt numFmtId="168" formatCode="0.0E+00"/>
   </numFmts>
-  <fonts count="29" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -452,39 +388,6 @@
       <name val="Calibri"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
       <sz val="10"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -494,48 +397,16 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
-    <font>
-      <b/>
-      <u/>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="10"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFBFBFBF"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="20">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -711,63 +582,6 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
   </borders>
@@ -788,7 +602,7 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="196">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1058,241 +872,26 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="15" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="21" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="21" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="21" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="1" fontId="20" fillId="2" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="168" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="21" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="21" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="20" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="25" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="20" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="20" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="11" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="26" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="26" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="165" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="23" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="1" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="2" fontId="27" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="23" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1633,8 +1232,8 @@
   </sheetPr>
   <dimension ref="B1:P93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2155,7 +1754,7 @@
         <v>39</v>
       </c>
       <c r="G27" s="89" t="s">
-        <v>97</v>
+        <v>76</v>
       </c>
       <c r="H27" s="16"/>
       <c r="I27" s="16"/>
@@ -2165,29 +1764,29 @@
       <c r="M27" s="21"/>
     </row>
     <row r="28" spans="2:13">
-      <c r="B28" s="122" t="s">
-        <v>85</v>
-      </c>
-      <c r="C28" s="131">
+      <c r="B28" s="105" t="s">
+        <v>75</v>
+      </c>
+      <c r="C28" s="108">
         <f>10^(E28/10)</f>
-        <v>6.3095734448019343</v>
-      </c>
-      <c r="D28" s="152"/>
-      <c r="E28" s="195">
-        <v>8</v>
-      </c>
-      <c r="F28" s="124" t="s">
+        <v>3.1622776601683795</v>
+      </c>
+      <c r="D28" s="109"/>
+      <c r="E28" s="110">
+        <v>5</v>
+      </c>
+      <c r="F28" s="106" t="s">
         <v>2</v>
       </c>
-      <c r="G28" s="106" t="s">
-        <v>98</v>
-      </c>
-      <c r="H28" s="106"/>
-      <c r="I28" s="106"/>
-      <c r="J28" s="106"/>
-      <c r="K28" s="106"/>
-      <c r="L28" s="105"/>
-      <c r="M28" s="126"/>
+      <c r="G28" s="104" t="s">
+        <v>77</v>
+      </c>
+      <c r="H28" s="103"/>
+      <c r="I28" s="103"/>
+      <c r="J28" s="103"/>
+      <c r="K28" s="103"/>
+      <c r="L28" s="102"/>
+      <c r="M28" s="107"/>
     </row>
     <row r="29" spans="2:13">
       <c r="B29" s="51" t="s">
@@ -2244,7 +1843,7 @@
       </c>
       <c r="C31" s="71">
         <f>$C$7*C27*(C30*1000)*C28</f>
-        <v>1.2631405980684847E-15</v>
+        <v>6.3306994202824191E-16</v>
       </c>
       <c r="D31" s="94" t="s">
         <v>7</v>
@@ -2535,12 +2134,12 @@
       </c>
       <c r="C44" s="80">
         <f>C42/C31</f>
-        <v>9.3441236331577859E-2</v>
+        <v>0.18643977751649826</v>
       </c>
       <c r="D44" s="78"/>
       <c r="E44" s="79">
         <f>10*LOG10(C44)</f>
-        <v>-10.294614239941977</v>
+        <v>-7.2946142399419758</v>
       </c>
       <c r="F44" s="78" t="s">
         <v>2</v>
@@ -2559,12 +2158,12 @@
       </c>
       <c r="C45" s="81">
         <f>C43/C31</f>
-        <v>47.841913001767864</v>
+        <v>95.45716608844711</v>
       </c>
       <c r="D45" s="78"/>
       <c r="E45" s="79">
         <f>10*LOG10(C45)</f>
-        <v>16.798085369816331</v>
+        <v>19.798085369816331</v>
       </c>
       <c r="F45" s="82" t="s">
         <v>2</v>
@@ -2582,12 +2181,12 @@
       </c>
       <c r="C46" s="84">
         <f>10^(E46/10)</f>
-        <v>4.7841913001767882</v>
+        <v>9.5457166088447103</v>
       </c>
       <c r="D46" s="85"/>
       <c r="E46" s="86">
         <f>E45-10</f>
-        <v>6.7980853698163308</v>
+        <v>9.7980853698163308</v>
       </c>
       <c r="F46" s="87" t="s">
         <v>2</v>
@@ -3275,13 +2874,13 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{DF438D20-ED32-4502-BBF3-1338727B4A2A}" showRuler="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <customSheetView guid="{56B56577-359B-4FEF-8511-5634C3B3AD8C}" showRuler="0">
+      <selection activeCell="L18" sqref="L18"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
-    <customSheetView guid="{56B56577-359B-4FEF-8511-5634C3B3AD8C}" showRuler="0">
-      <selection activeCell="L18" sqref="L18"/>
+    <customSheetView guid="{DF438D20-ED32-4502-BBF3-1338727B4A2A}" showRuler="0">
+      <selection activeCell="D24" sqref="D24"/>
       <pageSetup orientation="portrait"/>
       <headerFooter alignWithMargins="0"/>
     </customSheetView>
@@ -3311,1736 +2910,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:P99"/>
-  <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33:XFD33"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="2:16" ht="15">
-      <c r="B1" s="102" t="s">
-        <v>59</v>
-      </c>
-      <c r="C1" s="104"/>
-      <c r="D1" s="103"/>
-      <c r="E1" s="105"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="106"/>
-      <c r="I1" s="105"/>
-      <c r="J1" s="105"/>
-      <c r="K1" s="105"/>
-      <c r="L1" s="106"/>
-      <c r="M1" s="105"/>
-    </row>
-    <row r="2" spans="2:16" ht="15">
-      <c r="B2" s="102" t="s">
-        <v>75</v>
-      </c>
-      <c r="C2" s="104"/>
-      <c r="D2" s="103"/>
-      <c r="E2" s="105"/>
-      <c r="F2" s="105"/>
-      <c r="G2" s="106"/>
-      <c r="H2" s="106"/>
-      <c r="I2" s="105"/>
-      <c r="J2" s="105"/>
-      <c r="K2" s="105"/>
-      <c r="L2" s="106"/>
-      <c r="M2" s="105"/>
-    </row>
-    <row r="3" spans="2:16" ht="15">
-      <c r="B3" s="102" t="s">
-        <v>42</v>
-      </c>
-      <c r="C3" s="107"/>
-      <c r="D3" s="108"/>
-      <c r="E3" s="105"/>
-      <c r="F3" s="105"/>
-      <c r="G3" s="106"/>
-      <c r="H3" s="106"/>
-      <c r="I3" s="109"/>
-      <c r="J3" s="105"/>
-      <c r="K3" s="105"/>
-      <c r="L3" s="106"/>
-      <c r="M3" s="105"/>
-    </row>
-    <row r="4" spans="2:16" ht="14">
-      <c r="B4" s="110"/>
-      <c r="C4" s="107"/>
-      <c r="D4" s="111"/>
-      <c r="E4" s="105"/>
-      <c r="F4" s="105"/>
-      <c r="G4" s="106"/>
-      <c r="H4" s="106"/>
-      <c r="I4" s="109"/>
-      <c r="J4" s="105"/>
-      <c r="K4" s="105"/>
-      <c r="L4" s="106"/>
-      <c r="M4" s="105"/>
-    </row>
-    <row r="5" spans="2:16" ht="15" thickBot="1">
-      <c r="B5" s="112"/>
-      <c r="C5" s="106"/>
-      <c r="D5" s="113"/>
-      <c r="E5" s="113"/>
-      <c r="F5" s="113"/>
-      <c r="G5" s="113"/>
-      <c r="H5" s="106"/>
-      <c r="I5" s="105"/>
-      <c r="J5" s="105"/>
-      <c r="K5" s="105"/>
-      <c r="L5" s="106"/>
-      <c r="M5" s="115"/>
-      <c r="N5" s="114"/>
-      <c r="O5" s="114"/>
-      <c r="P5" s="114"/>
-    </row>
-    <row r="6" spans="2:16" ht="15" thickBot="1">
-      <c r="B6" s="116" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="117" t="s">
-        <v>37</v>
-      </c>
-      <c r="D6" s="118"/>
-      <c r="E6" s="119" t="s">
-        <v>22</v>
-      </c>
-      <c r="F6" s="120"/>
-      <c r="G6" s="121" t="s">
-        <v>76</v>
-      </c>
-      <c r="H6" s="106"/>
-      <c r="I6" s="105"/>
-      <c r="J6" s="113"/>
-      <c r="K6" s="113"/>
-      <c r="L6" s="113"/>
-      <c r="M6" s="105"/>
-    </row>
-    <row r="7" spans="2:16" ht="14">
-      <c r="B7" s="122" t="s">
-        <v>0</v>
-      </c>
-      <c r="C7" s="123">
-        <v>1.3809999999999999E-23</v>
-      </c>
-      <c r="D7" s="124" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7" s="125">
-        <v>-228.6</v>
-      </c>
-      <c r="F7" s="124" t="s">
-        <v>2</v>
-      </c>
-      <c r="G7" s="106"/>
-      <c r="H7" s="106"/>
-      <c r="I7" s="105"/>
-      <c r="J7" s="106"/>
-      <c r="K7" s="106"/>
-      <c r="L7" s="106"/>
-      <c r="M7" s="126"/>
-    </row>
-    <row r="8" spans="2:16" ht="14">
-      <c r="B8" s="122" t="s">
-        <v>3</v>
-      </c>
-      <c r="C8" s="127">
-        <v>300000000</v>
-      </c>
-      <c r="D8" s="124" t="s">
-        <v>4</v>
-      </c>
-      <c r="E8" s="125"/>
-      <c r="F8" s="124"/>
-      <c r="G8" s="106"/>
-      <c r="H8" s="106"/>
-      <c r="I8" s="105"/>
-      <c r="J8" s="106"/>
-      <c r="K8" s="106"/>
-      <c r="L8" s="106"/>
-      <c r="M8" s="126"/>
-    </row>
-    <row r="9" spans="2:16" ht="14">
-      <c r="B9" s="122" t="s">
-        <v>16</v>
-      </c>
-      <c r="C9" s="106">
-        <v>6378.14</v>
-      </c>
-      <c r="D9" s="124" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="125"/>
-      <c r="F9" s="124"/>
-      <c r="G9" s="106"/>
-      <c r="H9" s="106"/>
-      <c r="I9" s="105"/>
-      <c r="J9" s="106"/>
-      <c r="K9" s="106"/>
-      <c r="L9" s="106"/>
-      <c r="M9" s="126"/>
-    </row>
-    <row r="10" spans="2:16" ht="14">
-      <c r="B10" s="122" t="s">
-        <v>46</v>
-      </c>
-      <c r="C10" s="127">
-        <v>399000</v>
-      </c>
-      <c r="D10" s="124" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" s="125"/>
-      <c r="F10" s="124"/>
-      <c r="G10" s="106"/>
-      <c r="H10" s="106"/>
-      <c r="I10" s="105"/>
-      <c r="J10" s="106"/>
-      <c r="K10" s="106"/>
-      <c r="L10" s="106"/>
-      <c r="M10" s="126"/>
-    </row>
-    <row r="11" spans="2:16" ht="15" thickBot="1">
-      <c r="B11" s="122"/>
-      <c r="C11" s="106"/>
-      <c r="D11" s="124"/>
-      <c r="E11" s="125"/>
-      <c r="F11" s="124"/>
-      <c r="G11" s="106"/>
-      <c r="H11" s="106"/>
-      <c r="I11" s="105"/>
-      <c r="J11" s="106"/>
-      <c r="K11" s="106"/>
-      <c r="L11" s="106"/>
-      <c r="M11" s="126"/>
-    </row>
-    <row r="12" spans="2:16" ht="15" thickBot="1">
-      <c r="B12" s="116" t="s">
-        <v>44</v>
-      </c>
-      <c r="C12" s="117" t="s">
-        <v>37</v>
-      </c>
-      <c r="D12" s="118"/>
-      <c r="E12" s="119" t="s">
-        <v>22</v>
-      </c>
-      <c r="F12" s="120"/>
-      <c r="G12" s="121"/>
-      <c r="H12" s="106"/>
-      <c r="I12" s="105"/>
-      <c r="J12" s="106"/>
-      <c r="K12" s="106"/>
-      <c r="L12" s="106"/>
-      <c r="M12" s="126"/>
-    </row>
-    <row r="13" spans="2:16" ht="14">
-      <c r="B13" s="128" t="s">
-        <v>5</v>
-      </c>
-      <c r="C13" s="129">
-        <v>902</v>
-      </c>
-      <c r="D13" s="130" t="s">
-        <v>11</v>
-      </c>
-      <c r="E13" s="125"/>
-      <c r="F13" s="124"/>
-      <c r="G13" s="106"/>
-      <c r="H13" s="106"/>
-      <c r="I13" s="105"/>
-      <c r="J13" s="125"/>
-      <c r="K13" s="125"/>
-      <c r="L13" s="106"/>
-      <c r="M13" s="126"/>
-    </row>
-    <row r="14" spans="2:16" ht="14">
-      <c r="B14" s="122" t="s">
-        <v>25</v>
-      </c>
-      <c r="C14" s="131">
-        <v>0.33300000000000002</v>
-      </c>
-      <c r="D14" s="124" t="s">
-        <v>19</v>
-      </c>
-      <c r="E14" s="125"/>
-      <c r="F14" s="124"/>
-      <c r="G14" s="106"/>
-      <c r="H14" s="106"/>
-      <c r="I14" s="105"/>
-      <c r="J14" s="106"/>
-      <c r="K14" s="106"/>
-      <c r="L14" s="106"/>
-      <c r="M14" s="126"/>
-    </row>
-    <row r="15" spans="2:16" ht="15" thickBot="1">
-      <c r="B15" s="122"/>
-      <c r="C15" s="106"/>
-      <c r="D15" s="124"/>
-      <c r="E15" s="106"/>
-      <c r="F15" s="124"/>
-      <c r="G15" s="106"/>
-      <c r="H15" s="106"/>
-      <c r="I15" s="105"/>
-      <c r="J15" s="106"/>
-      <c r="K15" s="106"/>
-      <c r="L15" s="106"/>
-      <c r="M15" s="126"/>
-    </row>
-    <row r="16" spans="2:16" ht="15" thickBot="1">
-      <c r="B16" s="116" t="s">
-        <v>45</v>
-      </c>
-      <c r="C16" s="117"/>
-      <c r="D16" s="118"/>
-      <c r="E16" s="119"/>
-      <c r="F16" s="120"/>
-      <c r="G16" s="121"/>
-      <c r="H16" s="106"/>
-      <c r="I16" s="105"/>
-      <c r="J16" s="106"/>
-      <c r="K16" s="106"/>
-      <c r="L16" s="106"/>
-      <c r="M16" s="126"/>
-    </row>
-    <row r="17" spans="2:13" ht="14">
-      <c r="B17" s="128" t="s">
-        <v>18</v>
-      </c>
-      <c r="C17" s="132">
-        <v>600</v>
-      </c>
-      <c r="D17" s="130" t="s">
-        <v>12</v>
-      </c>
-      <c r="E17" s="125"/>
-      <c r="F17" s="124"/>
-      <c r="G17" s="106"/>
-      <c r="H17" s="106"/>
-      <c r="I17" s="105"/>
-      <c r="J17" s="106"/>
-      <c r="K17" s="106"/>
-      <c r="L17" s="106"/>
-      <c r="M17" s="126"/>
-    </row>
-    <row r="18" spans="2:13" ht="14">
-      <c r="B18" s="128" t="s">
-        <v>63</v>
-      </c>
-      <c r="C18" s="133">
-        <v>60</v>
-      </c>
-      <c r="D18" s="130" t="s">
-        <v>17</v>
-      </c>
-      <c r="E18" s="106"/>
-      <c r="F18" s="124"/>
-      <c r="G18" s="106"/>
-      <c r="H18" s="106"/>
-      <c r="I18" s="105"/>
-      <c r="J18" s="106"/>
-      <c r="K18" s="106"/>
-      <c r="L18" s="106"/>
-      <c r="M18" s="126"/>
-    </row>
-    <row r="19" spans="2:13" ht="14">
-      <c r="B19" s="122" t="s">
-        <v>23</v>
-      </c>
-      <c r="C19" s="134">
-        <v>683.2</v>
-      </c>
-      <c r="D19" s="124" t="s">
-        <v>12</v>
-      </c>
-      <c r="E19" s="125"/>
-      <c r="F19" s="124"/>
-      <c r="G19" s="106"/>
-      <c r="H19" s="106"/>
-      <c r="I19" s="105"/>
-      <c r="J19" s="106"/>
-      <c r="K19" s="106"/>
-      <c r="L19" s="106"/>
-      <c r="M19" s="126"/>
-    </row>
-    <row r="20" spans="2:13" ht="14">
-      <c r="B20" s="122" t="s">
-        <v>54</v>
-      </c>
-      <c r="C20" s="134">
-        <v>96.7</v>
-      </c>
-      <c r="D20" s="124" t="s">
-        <v>55</v>
-      </c>
-      <c r="E20" s="106"/>
-      <c r="F20" s="124"/>
-      <c r="G20" s="109" t="s">
-        <v>77</v>
-      </c>
-      <c r="H20" s="106"/>
-      <c r="I20" s="105"/>
-      <c r="J20" s="106"/>
-      <c r="K20" s="106"/>
-      <c r="L20" s="106"/>
-      <c r="M20" s="126"/>
-    </row>
-    <row r="21" spans="2:13" ht="14">
-      <c r="B21" s="122" t="s">
-        <v>78</v>
-      </c>
-      <c r="C21" s="134">
-        <v>1.5</v>
-      </c>
-      <c r="D21" s="124" t="s">
-        <v>55</v>
-      </c>
-      <c r="E21" s="106"/>
-      <c r="F21" s="124"/>
-      <c r="G21" s="109" t="s">
-        <v>79</v>
-      </c>
-      <c r="H21" s="106"/>
-      <c r="I21" s="105"/>
-      <c r="J21" s="106"/>
-      <c r="K21" s="106"/>
-      <c r="L21" s="106"/>
-      <c r="M21" s="126"/>
-    </row>
-    <row r="22" spans="2:13" ht="14">
-      <c r="B22" s="122" t="s">
-        <v>53</v>
-      </c>
-      <c r="C22" s="134">
-        <v>7.6</v>
-      </c>
-      <c r="D22" s="124" t="s">
-        <v>48</v>
-      </c>
-      <c r="E22" s="125"/>
-      <c r="F22" s="124"/>
-      <c r="G22" s="109" t="s">
-        <v>80</v>
-      </c>
-      <c r="H22" s="106"/>
-      <c r="I22" s="105"/>
-      <c r="J22" s="106"/>
-      <c r="K22" s="106"/>
-      <c r="L22" s="106"/>
-      <c r="M22" s="126"/>
-    </row>
-    <row r="23" spans="2:13" ht="14">
-      <c r="B23" s="122" t="s">
-        <v>52</v>
-      </c>
-      <c r="C23" s="134">
-        <v>3.8</v>
-      </c>
-      <c r="D23" s="124" t="s">
-        <v>48</v>
-      </c>
-      <c r="E23" s="125"/>
-      <c r="F23" s="124"/>
-      <c r="G23" s="109" t="s">
-        <v>81</v>
-      </c>
-      <c r="H23" s="106"/>
-      <c r="I23" s="105"/>
-      <c r="J23" s="106"/>
-      <c r="K23" s="106"/>
-      <c r="L23" s="106"/>
-      <c r="M23" s="126"/>
-    </row>
-    <row r="24" spans="2:13" ht="14">
-      <c r="B24" s="122" t="s">
-        <v>51</v>
-      </c>
-      <c r="C24" s="134">
-        <v>11.4</v>
-      </c>
-      <c r="D24" s="124" t="s">
-        <v>49</v>
-      </c>
-      <c r="E24" s="125"/>
-      <c r="F24" s="124"/>
-      <c r="G24" s="109" t="s">
-        <v>82</v>
-      </c>
-      <c r="H24" s="106"/>
-      <c r="I24" s="105"/>
-      <c r="J24" s="106"/>
-      <c r="K24" s="106"/>
-      <c r="L24" s="106"/>
-      <c r="M24" s="126"/>
-    </row>
-    <row r="25" spans="2:13" ht="15" thickBot="1">
-      <c r="B25" s="122"/>
-      <c r="C25" s="134"/>
-      <c r="D25" s="124"/>
-      <c r="E25" s="125"/>
-      <c r="F25" s="124"/>
-      <c r="G25" s="106"/>
-      <c r="H25" s="106"/>
-      <c r="I25" s="105"/>
-      <c r="J25" s="106"/>
-      <c r="K25" s="106"/>
-      <c r="L25" s="106"/>
-      <c r="M25" s="126"/>
-    </row>
-    <row r="26" spans="2:13" ht="15" thickBot="1">
-      <c r="B26" s="116" t="s">
-        <v>24</v>
-      </c>
-      <c r="C26" s="117"/>
-      <c r="D26" s="118"/>
-      <c r="E26" s="119"/>
-      <c r="F26" s="120"/>
-      <c r="G26" s="121"/>
-      <c r="H26" s="106"/>
-      <c r="I26" s="106"/>
-      <c r="J26" s="105"/>
-      <c r="K26" s="106"/>
-      <c r="L26" s="106"/>
-      <c r="M26" s="126"/>
-    </row>
-    <row r="27" spans="2:13" ht="14">
-      <c r="B27" s="122" t="s">
-        <v>10</v>
-      </c>
-      <c r="C27" s="135">
-        <v>1.4999999999999999E-15</v>
-      </c>
-      <c r="D27" s="124"/>
-      <c r="E27" s="134">
-        <v>-148.30000000000001</v>
-      </c>
-      <c r="F27" s="124" t="s">
-        <v>2</v>
-      </c>
-      <c r="G27" s="136" t="s">
-        <v>83</v>
-      </c>
-      <c r="H27" s="136"/>
-      <c r="I27" s="105"/>
-      <c r="J27" s="105"/>
-      <c r="K27" s="106"/>
-      <c r="L27" s="106"/>
-      <c r="M27" s="126"/>
-    </row>
-    <row r="28" spans="2:13" ht="14">
-      <c r="B28" s="122" t="s">
-        <v>27</v>
-      </c>
-      <c r="C28" s="131">
-        <v>0.63100000000000001</v>
-      </c>
-      <c r="D28" s="106"/>
-      <c r="E28" s="137">
-        <v>-2</v>
-      </c>
-      <c r="F28" s="124" t="s">
-        <v>2</v>
-      </c>
-      <c r="G28" s="138"/>
-      <c r="H28" s="106"/>
-      <c r="I28" s="105"/>
-      <c r="J28" s="105"/>
-      <c r="K28" s="125"/>
-      <c r="L28" s="106"/>
-      <c r="M28" s="126"/>
-    </row>
-    <row r="29" spans="2:13" ht="15" thickBot="1">
-      <c r="B29" s="139"/>
-      <c r="C29" s="140"/>
-      <c r="D29" s="141"/>
-      <c r="E29" s="142"/>
-      <c r="F29" s="141"/>
-      <c r="G29" s="106"/>
-      <c r="H29" s="106"/>
-      <c r="I29" s="125"/>
-      <c r="J29" s="105"/>
-      <c r="K29" s="106"/>
-      <c r="L29" s="106"/>
-      <c r="M29" s="126"/>
-    </row>
-    <row r="30" spans="2:13" ht="15" thickBot="1">
-      <c r="B30" s="143" t="s">
-        <v>13</v>
-      </c>
-      <c r="C30" s="144"/>
-      <c r="D30" s="145"/>
-      <c r="E30" s="146"/>
-      <c r="F30" s="147"/>
-      <c r="G30" s="121"/>
-      <c r="H30" s="106"/>
-      <c r="I30" s="106"/>
-      <c r="J30" s="106"/>
-      <c r="K30" s="106"/>
-      <c r="L30" s="105"/>
-      <c r="M30" s="126"/>
-    </row>
-    <row r="31" spans="2:13" ht="14">
-      <c r="B31" s="128" t="s">
-        <v>9</v>
-      </c>
-      <c r="C31" s="148">
-        <v>50.12</v>
-      </c>
-      <c r="D31" s="149"/>
-      <c r="E31" s="150">
-        <v>17</v>
-      </c>
-      <c r="F31" s="130" t="s">
-        <v>2</v>
-      </c>
-      <c r="G31" s="121"/>
-      <c r="H31" s="106"/>
-      <c r="I31" s="106"/>
-      <c r="J31" s="106"/>
-      <c r="K31" s="106"/>
-      <c r="L31" s="105"/>
-      <c r="M31" s="126"/>
-    </row>
-    <row r="32" spans="2:13" ht="14">
-      <c r="B32" s="122" t="s">
-        <v>84</v>
-      </c>
-      <c r="C32" s="125">
-        <v>290</v>
-      </c>
-      <c r="D32" s="124" t="s">
-        <v>20</v>
-      </c>
-      <c r="E32" s="151">
-        <v>24.6</v>
-      </c>
-      <c r="F32" s="124" t="s">
-        <v>39</v>
-      </c>
-      <c r="G32" s="121"/>
-      <c r="H32" s="106"/>
-      <c r="I32" s="106"/>
-      <c r="J32" s="106"/>
-      <c r="K32" s="106"/>
-      <c r="L32" s="105"/>
-      <c r="M32" s="126"/>
-    </row>
-    <row r="33" spans="2:13" ht="14">
-      <c r="B33" s="122" t="s">
-        <v>85</v>
-      </c>
-      <c r="C33" s="131">
-        <v>1.151</v>
-      </c>
-      <c r="D33" s="152"/>
-      <c r="E33" s="153">
-        <v>0.61</v>
-      </c>
-      <c r="F33" s="124" t="s">
-        <v>2</v>
-      </c>
-      <c r="G33" s="106"/>
-      <c r="H33" s="106"/>
-      <c r="I33" s="106"/>
-      <c r="J33" s="106"/>
-      <c r="K33" s="106"/>
-      <c r="L33" s="105"/>
-      <c r="M33" s="126"/>
-    </row>
-    <row r="34" spans="2:13" ht="14">
-      <c r="B34" s="122" t="s">
-        <v>38</v>
-      </c>
-      <c r="C34" s="125">
-        <v>0.5</v>
-      </c>
-      <c r="D34" s="124"/>
-      <c r="E34" s="151">
-        <v>-3</v>
-      </c>
-      <c r="F34" s="124" t="s">
-        <v>2</v>
-      </c>
-      <c r="G34" s="121"/>
-      <c r="H34" s="106"/>
-      <c r="I34" s="106"/>
-      <c r="J34" s="106"/>
-      <c r="K34" s="106"/>
-      <c r="L34" s="105"/>
-      <c r="M34" s="126"/>
-    </row>
-    <row r="35" spans="2:13" ht="14">
-      <c r="B35" s="122" t="s">
-        <v>28</v>
-      </c>
-      <c r="C35" s="154">
-        <v>100</v>
-      </c>
-      <c r="D35" s="124" t="s">
-        <v>49</v>
-      </c>
-      <c r="E35" s="134">
-        <v>50</v>
-      </c>
-      <c r="F35" s="124" t="s">
-        <v>8</v>
-      </c>
-      <c r="G35" s="155" t="s">
-        <v>86</v>
-      </c>
-      <c r="H35" s="106"/>
-      <c r="I35" s="106"/>
-      <c r="J35" s="106"/>
-      <c r="K35" s="106"/>
-      <c r="L35" s="105"/>
-      <c r="M35" s="126"/>
-    </row>
-    <row r="36" spans="2:13" ht="14">
-      <c r="B36" s="122" t="s">
-        <v>87</v>
-      </c>
-      <c r="C36" s="127">
-        <v>4.61E-16</v>
-      </c>
-      <c r="D36" s="124" t="s">
-        <v>7</v>
-      </c>
-      <c r="E36" s="125">
-        <v>-153.37</v>
-      </c>
-      <c r="F36" s="124" t="s">
-        <v>6</v>
-      </c>
-      <c r="G36" s="126" t="s">
-        <v>88</v>
-      </c>
-      <c r="H36" s="106"/>
-      <c r="I36" s="106"/>
-      <c r="J36" s="106"/>
-      <c r="K36" s="106"/>
-      <c r="L36" s="105"/>
-      <c r="M36" s="126"/>
-    </row>
-    <row r="37" spans="2:13" ht="15" thickBot="1">
-      <c r="B37" s="139"/>
-      <c r="C37" s="140"/>
-      <c r="D37" s="141"/>
-      <c r="E37" s="142"/>
-      <c r="F37" s="141"/>
-      <c r="G37" s="121"/>
-      <c r="H37" s="106"/>
-      <c r="I37" s="106"/>
-      <c r="J37" s="106"/>
-      <c r="K37" s="106"/>
-      <c r="L37" s="105"/>
-      <c r="M37" s="126"/>
-    </row>
-    <row r="38" spans="2:13" ht="15" thickBot="1">
-      <c r="B38" s="143" t="s">
-        <v>40</v>
-      </c>
-      <c r="C38" s="144"/>
-      <c r="D38" s="145"/>
-      <c r="E38" s="146"/>
-      <c r="F38" s="147"/>
-      <c r="G38" s="121"/>
-      <c r="H38" s="106"/>
-      <c r="I38" s="106"/>
-      <c r="J38" s="106"/>
-      <c r="K38" s="106"/>
-      <c r="L38" s="105"/>
-      <c r="M38" s="126"/>
-    </row>
-    <row r="39" spans="2:13" ht="14">
-      <c r="B39" s="156" t="s">
-        <v>26</v>
-      </c>
-      <c r="C39" s="157">
-        <v>1.26</v>
-      </c>
-      <c r="D39" s="149"/>
-      <c r="E39" s="158">
-        <v>1</v>
-      </c>
-      <c r="F39" s="130" t="s">
-        <v>2</v>
-      </c>
-      <c r="G39" s="121"/>
-      <c r="H39" s="106"/>
-      <c r="I39" s="106"/>
-      <c r="J39" s="106"/>
-      <c r="K39" s="106"/>
-      <c r="L39" s="105"/>
-      <c r="M39" s="126"/>
-    </row>
-    <row r="40" spans="2:13" ht="14">
-      <c r="B40" s="159" t="s">
-        <v>89</v>
-      </c>
-      <c r="C40" s="160">
-        <v>0.79400000000000004</v>
-      </c>
-      <c r="D40" s="152"/>
-      <c r="E40" s="161">
-        <v>-1</v>
-      </c>
-      <c r="F40" s="124" t="s">
-        <v>2</v>
-      </c>
-      <c r="G40" s="106"/>
-      <c r="H40" s="106"/>
-      <c r="I40" s="106"/>
-      <c r="J40" s="106"/>
-      <c r="K40" s="106"/>
-      <c r="L40" s="105"/>
-      <c r="M40" s="126"/>
-    </row>
-    <row r="41" spans="2:13" ht="14">
-      <c r="B41" s="159" t="s">
-        <v>34</v>
-      </c>
-      <c r="C41" s="162">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="D41" s="124" t="s">
-        <v>7</v>
-      </c>
-      <c r="E41" s="125">
-        <v>-19.59</v>
-      </c>
-      <c r="F41" s="124" t="s">
-        <v>15</v>
-      </c>
-      <c r="G41" s="121"/>
-      <c r="H41" s="106"/>
-      <c r="I41" s="106"/>
-      <c r="J41" s="106"/>
-      <c r="K41" s="106"/>
-      <c r="L41" s="105"/>
-      <c r="M41" s="126"/>
-    </row>
-    <row r="42" spans="2:13" ht="14">
-      <c r="B42" s="159" t="s">
-        <v>43</v>
-      </c>
-      <c r="C42" s="160">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="D42" s="124" t="s">
-        <v>7</v>
-      </c>
-      <c r="E42" s="125">
-        <v>-19.59</v>
-      </c>
-      <c r="F42" s="124" t="s">
-        <v>15</v>
-      </c>
-      <c r="G42" s="121"/>
-      <c r="H42" s="106"/>
-      <c r="I42" s="125"/>
-      <c r="J42" s="105"/>
-      <c r="K42" s="106"/>
-      <c r="L42" s="106"/>
-      <c r="M42" s="126"/>
-    </row>
-    <row r="43" spans="2:13" ht="15" thickBot="1">
-      <c r="B43" s="163"/>
-      <c r="C43" s="164"/>
-      <c r="D43" s="141"/>
-      <c r="E43" s="142"/>
-      <c r="F43" s="141"/>
-      <c r="G43" s="121"/>
-      <c r="H43" s="106"/>
-      <c r="I43" s="125"/>
-      <c r="J43" s="105"/>
-      <c r="K43" s="106"/>
-      <c r="L43" s="106"/>
-      <c r="M43" s="126"/>
-    </row>
-    <row r="44" spans="2:13" ht="15" thickBot="1">
-      <c r="B44" s="143" t="s">
-        <v>56</v>
-      </c>
-      <c r="C44" s="144"/>
-      <c r="D44" s="145"/>
-      <c r="E44" s="146"/>
-      <c r="F44" s="147"/>
-      <c r="G44" s="121"/>
-      <c r="H44" s="106"/>
-      <c r="I44" s="125"/>
-      <c r="J44" s="105"/>
-      <c r="K44" s="106"/>
-      <c r="L44" s="106"/>
-      <c r="M44" s="126"/>
-    </row>
-    <row r="45" spans="2:13" ht="14">
-      <c r="B45" s="122" t="s">
-        <v>32</v>
-      </c>
-      <c r="C45" s="165">
-        <v>50</v>
-      </c>
-      <c r="D45" s="124" t="s">
-        <v>50</v>
-      </c>
-      <c r="E45" s="125"/>
-      <c r="F45" s="124"/>
-      <c r="G45" s="106"/>
-      <c r="H45" s="106"/>
-      <c r="I45" s="125"/>
-      <c r="J45" s="105"/>
-      <c r="K45" s="106"/>
-      <c r="L45" s="106"/>
-      <c r="M45" s="126"/>
-    </row>
-    <row r="46" spans="2:13" ht="14">
-      <c r="B46" s="122" t="s">
-        <v>90</v>
-      </c>
-      <c r="C46" s="166">
-        <v>0.01</v>
-      </c>
-      <c r="D46" s="124" t="s">
-        <v>91</v>
-      </c>
-      <c r="E46" s="125"/>
-      <c r="F46" s="124"/>
-      <c r="G46" s="106"/>
-      <c r="H46" s="106"/>
-      <c r="I46" s="125"/>
-      <c r="J46" s="105"/>
-      <c r="K46" s="106"/>
-      <c r="L46" s="106"/>
-      <c r="M46" s="126"/>
-    </row>
-    <row r="47" spans="2:13" ht="14">
-      <c r="B47" s="122" t="s">
-        <v>31</v>
-      </c>
-      <c r="C47" s="125">
-        <v>0.1</v>
-      </c>
-      <c r="D47" s="106" t="s">
-        <v>49</v>
-      </c>
-      <c r="E47" s="167"/>
-      <c r="F47" s="124"/>
-      <c r="G47" s="138"/>
-      <c r="H47" s="106"/>
-      <c r="I47" s="125"/>
-      <c r="J47" s="105"/>
-      <c r="K47" s="106"/>
-      <c r="L47" s="106"/>
-      <c r="M47" s="126"/>
-    </row>
-    <row r="48" spans="2:13" ht="14">
-      <c r="B48" s="122" t="s">
-        <v>92</v>
-      </c>
-      <c r="C48" s="106">
-        <v>511</v>
-      </c>
-      <c r="D48" s="106"/>
-      <c r="E48" s="167"/>
-      <c r="F48" s="124"/>
-      <c r="G48" s="138"/>
-      <c r="H48" s="106"/>
-      <c r="I48" s="125"/>
-      <c r="J48" s="105"/>
-      <c r="K48" s="106"/>
-      <c r="L48" s="106"/>
-      <c r="M48" s="126"/>
-    </row>
-    <row r="49" spans="2:13" ht="14">
-      <c r="B49" s="122" t="s">
-        <v>30</v>
-      </c>
-      <c r="C49" s="125">
-        <v>511</v>
-      </c>
-      <c r="D49" s="124"/>
-      <c r="E49" s="125">
-        <v>27.08</v>
-      </c>
-      <c r="F49" s="124" t="s">
-        <v>2</v>
-      </c>
-      <c r="G49" s="138" t="s">
-        <v>93</v>
-      </c>
-      <c r="H49" s="106"/>
-      <c r="I49" s="125"/>
-      <c r="J49" s="105"/>
-      <c r="K49" s="106"/>
-      <c r="L49" s="106"/>
-      <c r="M49" s="126"/>
-    </row>
-    <row r="50" spans="2:13" ht="15" thickBot="1">
-      <c r="B50" s="139"/>
-      <c r="C50" s="140"/>
-      <c r="D50" s="141"/>
-      <c r="E50" s="142"/>
-      <c r="F50" s="141"/>
-      <c r="G50" s="106"/>
-      <c r="H50" s="106"/>
-      <c r="I50" s="125"/>
-      <c r="J50" s="105"/>
-      <c r="K50" s="106"/>
-      <c r="L50" s="106"/>
-      <c r="M50" s="126"/>
-    </row>
-    <row r="51" spans="2:13" ht="15" thickBot="1">
-      <c r="B51" s="143" t="s">
-        <v>41</v>
-      </c>
-      <c r="C51" s="144"/>
-      <c r="D51" s="145"/>
-      <c r="E51" s="146"/>
-      <c r="F51" s="147"/>
-      <c r="G51" s="121"/>
-      <c r="H51" s="106"/>
-      <c r="I51" s="125"/>
-      <c r="J51" s="105"/>
-      <c r="K51" s="106"/>
-      <c r="L51" s="106"/>
-      <c r="M51" s="126"/>
-    </row>
-    <row r="52" spans="2:13" ht="14">
-      <c r="B52" s="168" t="s">
-        <v>94</v>
-      </c>
-      <c r="C52" s="169">
-        <v>3.2900000000000002E-16</v>
-      </c>
-      <c r="D52" s="170" t="s">
-        <v>7</v>
-      </c>
-      <c r="E52" s="171">
-        <v>-154.84</v>
-      </c>
-      <c r="F52" s="170" t="s">
-        <v>6</v>
-      </c>
-      <c r="G52" s="106"/>
-      <c r="H52" s="106"/>
-      <c r="I52" s="125"/>
-      <c r="J52" s="105"/>
-      <c r="K52" s="106"/>
-      <c r="L52" s="106"/>
-      <c r="M52" s="126"/>
-    </row>
-    <row r="53" spans="2:13" ht="14">
-      <c r="B53" s="168" t="s">
-        <v>58</v>
-      </c>
-      <c r="C53" s="169">
-        <v>1.6799999999999999E-13</v>
-      </c>
-      <c r="D53" s="170" t="s">
-        <v>7</v>
-      </c>
-      <c r="E53" s="172">
-        <v>-127.75</v>
-      </c>
-      <c r="F53" s="170" t="s">
-        <v>6</v>
-      </c>
-      <c r="G53" s="106"/>
-      <c r="H53" s="106"/>
-      <c r="I53" s="125"/>
-      <c r="J53" s="105"/>
-      <c r="K53" s="106"/>
-      <c r="L53" s="106"/>
-      <c r="M53" s="126"/>
-    </row>
-    <row r="54" spans="2:13" ht="14">
-      <c r="B54" s="168" t="s">
-        <v>35</v>
-      </c>
-      <c r="C54" s="173">
-        <v>0.71499999999999997</v>
-      </c>
-      <c r="D54" s="170"/>
-      <c r="E54" s="172">
-        <v>-1.46</v>
-      </c>
-      <c r="F54" s="170" t="s">
-        <v>2</v>
-      </c>
-      <c r="G54" s="126" t="s">
-        <v>95</v>
-      </c>
-      <c r="H54" s="106"/>
-      <c r="I54" s="125"/>
-      <c r="J54" s="105"/>
-      <c r="K54" s="106"/>
-      <c r="L54" s="106"/>
-      <c r="M54" s="126"/>
-    </row>
-    <row r="55" spans="2:13" ht="14">
-      <c r="B55" s="174" t="s">
-        <v>36</v>
-      </c>
-      <c r="C55" s="175">
-        <v>365.3</v>
-      </c>
-      <c r="D55" s="176"/>
-      <c r="E55" s="177">
-        <v>25.63</v>
-      </c>
-      <c r="F55" s="176" t="s">
-        <v>2</v>
-      </c>
-      <c r="G55" s="126" t="s">
-        <v>96</v>
-      </c>
-      <c r="H55" s="106"/>
-      <c r="I55" s="125"/>
-      <c r="J55" s="105"/>
-      <c r="K55" s="106"/>
-      <c r="L55" s="106"/>
-      <c r="M55" s="126"/>
-    </row>
-    <row r="56" spans="2:13" ht="14">
-      <c r="B56" s="174" t="s">
-        <v>33</v>
-      </c>
-      <c r="C56" s="177">
-        <v>36.53</v>
-      </c>
-      <c r="D56" s="149"/>
-      <c r="E56" s="177">
-        <v>15.63</v>
-      </c>
-      <c r="F56" s="176" t="s">
-        <v>2</v>
-      </c>
-      <c r="G56" s="178"/>
-      <c r="H56" s="106"/>
-      <c r="I56" s="125"/>
-      <c r="J56" s="105"/>
-      <c r="K56" s="106"/>
-      <c r="L56" s="106"/>
-      <c r="M56" s="126"/>
-    </row>
-    <row r="57" spans="2:13" ht="15" thickBot="1">
-      <c r="B57" s="139"/>
-      <c r="C57" s="179"/>
-      <c r="D57" s="180"/>
-      <c r="E57" s="181"/>
-      <c r="F57" s="182"/>
-      <c r="G57" s="106"/>
-      <c r="H57" s="106"/>
-      <c r="I57" s="125"/>
-      <c r="J57" s="105"/>
-      <c r="K57" s="106"/>
-      <c r="L57" s="106"/>
-      <c r="M57" s="126"/>
-    </row>
-    <row r="58" spans="2:13" ht="14">
-      <c r="B58" s="109"/>
-      <c r="C58" s="183"/>
-      <c r="D58" s="184"/>
-      <c r="E58" s="105"/>
-      <c r="F58" s="106"/>
-      <c r="G58" s="106"/>
-      <c r="H58" s="106"/>
-      <c r="I58" s="125"/>
-      <c r="J58" s="105"/>
-      <c r="K58" s="106"/>
-      <c r="L58" s="106"/>
-      <c r="M58" s="126"/>
-    </row>
-    <row r="59" spans="2:13" ht="14">
-      <c r="B59" s="185"/>
-      <c r="C59" s="186"/>
-      <c r="D59" s="115"/>
-      <c r="E59" s="186"/>
-      <c r="F59" s="115"/>
-      <c r="G59" s="109"/>
-      <c r="H59" s="106"/>
-      <c r="I59" s="125"/>
-      <c r="J59" s="105"/>
-      <c r="K59" s="106"/>
-      <c r="L59" s="106"/>
-      <c r="M59" s="126"/>
-    </row>
-    <row r="60" spans="2:13" ht="14">
-      <c r="B60" s="109"/>
-      <c r="C60" s="134"/>
-      <c r="D60" s="106"/>
-      <c r="E60" s="125"/>
-      <c r="F60" s="106"/>
-      <c r="G60" s="106"/>
-      <c r="H60" s="106"/>
-      <c r="I60" s="125"/>
-      <c r="J60" s="105"/>
-      <c r="K60" s="106"/>
-      <c r="L60" s="106"/>
-      <c r="M60" s="126"/>
-    </row>
-    <row r="61" spans="2:13" ht="14">
-      <c r="B61" s="185"/>
-      <c r="C61" s="187"/>
-      <c r="D61" s="115"/>
-      <c r="E61" s="186"/>
-      <c r="F61" s="115"/>
-      <c r="G61" s="106"/>
-      <c r="H61" s="106"/>
-      <c r="I61" s="125"/>
-      <c r="J61" s="105"/>
-      <c r="K61" s="106"/>
-      <c r="L61" s="106"/>
-      <c r="M61" s="126"/>
-    </row>
-    <row r="62" spans="2:13" ht="14">
-      <c r="B62" s="109"/>
-      <c r="C62" s="134"/>
-      <c r="D62" s="106"/>
-      <c r="E62" s="125"/>
-      <c r="F62" s="106"/>
-      <c r="G62" s="106"/>
-      <c r="H62" s="106"/>
-      <c r="I62" s="125"/>
-      <c r="J62" s="105"/>
-      <c r="K62" s="106"/>
-      <c r="L62" s="106"/>
-      <c r="M62" s="126"/>
-    </row>
-    <row r="63" spans="2:13" ht="14">
-      <c r="B63" s="109"/>
-      <c r="C63" s="134"/>
-      <c r="D63" s="106"/>
-      <c r="E63" s="125"/>
-      <c r="F63" s="106"/>
-      <c r="G63" s="106"/>
-      <c r="H63" s="106"/>
-      <c r="I63" s="125"/>
-      <c r="J63" s="105"/>
-      <c r="K63" s="106"/>
-      <c r="L63" s="106"/>
-      <c r="M63" s="126"/>
-    </row>
-    <row r="64" spans="2:13" ht="14">
-      <c r="B64" s="188"/>
-      <c r="C64" s="125"/>
-      <c r="D64" s="125"/>
-      <c r="E64" s="125"/>
-      <c r="F64" s="125"/>
-      <c r="G64" s="106"/>
-      <c r="H64" s="125"/>
-      <c r="I64" s="125"/>
-      <c r="J64" s="125"/>
-      <c r="K64" s="125"/>
-      <c r="L64" s="106"/>
-      <c r="M64" s="126"/>
-    </row>
-    <row r="65" spans="2:13" ht="14">
-      <c r="B65" s="109"/>
-      <c r="C65" s="106"/>
-      <c r="D65" s="106"/>
-      <c r="E65" s="105"/>
-      <c r="F65" s="106"/>
-      <c r="G65" s="106"/>
-      <c r="H65" s="134"/>
-      <c r="I65" s="134"/>
-      <c r="J65" s="105"/>
-      <c r="K65" s="134"/>
-      <c r="L65" s="106"/>
-      <c r="M65" s="126"/>
-    </row>
-    <row r="66" spans="2:13" ht="14">
-      <c r="B66" s="109"/>
-      <c r="C66" s="127"/>
-      <c r="D66" s="127"/>
-      <c r="E66" s="105"/>
-      <c r="F66" s="127"/>
-      <c r="G66" s="106"/>
-      <c r="H66" s="125"/>
-      <c r="I66" s="125"/>
-      <c r="J66" s="105"/>
-      <c r="K66" s="125"/>
-      <c r="L66" s="106"/>
-      <c r="M66" s="105"/>
-    </row>
-    <row r="67" spans="2:13" ht="14">
-      <c r="B67" s="109"/>
-      <c r="C67" s="127"/>
-      <c r="D67" s="127"/>
-      <c r="E67" s="127"/>
-      <c r="F67" s="127"/>
-      <c r="G67" s="106"/>
-      <c r="H67" s="125"/>
-      <c r="I67" s="125"/>
-      <c r="J67" s="125"/>
-      <c r="K67" s="125"/>
-      <c r="L67" s="106"/>
-      <c r="M67" s="126"/>
-    </row>
-    <row r="68" spans="2:13" ht="14">
-      <c r="B68" s="188"/>
-      <c r="C68" s="106"/>
-      <c r="D68" s="106"/>
-      <c r="E68" s="105"/>
-      <c r="F68" s="106"/>
-      <c r="G68" s="106"/>
-      <c r="H68" s="106"/>
-      <c r="I68" s="106"/>
-      <c r="J68" s="105"/>
-      <c r="K68" s="106"/>
-      <c r="L68" s="106"/>
-      <c r="M68" s="126"/>
-    </row>
-    <row r="69" spans="2:13" ht="14">
-      <c r="B69" s="109"/>
-      <c r="C69" s="125"/>
-      <c r="D69" s="125"/>
-      <c r="E69" s="105"/>
-      <c r="F69" s="125"/>
-      <c r="G69" s="106"/>
-      <c r="H69" s="125"/>
-      <c r="I69" s="125"/>
-      <c r="J69" s="105"/>
-      <c r="K69" s="125"/>
-      <c r="L69" s="106"/>
-      <c r="M69" s="178"/>
-    </row>
-    <row r="70" spans="2:13" ht="14">
-      <c r="B70" s="109"/>
-      <c r="C70" s="169"/>
-      <c r="D70" s="169"/>
-      <c r="E70" s="105"/>
-      <c r="F70" s="169"/>
-      <c r="G70" s="106"/>
-      <c r="H70" s="186"/>
-      <c r="I70" s="186"/>
-      <c r="J70" s="105"/>
-      <c r="K70" s="186"/>
-      <c r="L70" s="106"/>
-      <c r="M70" s="105"/>
-    </row>
-    <row r="71" spans="2:13" ht="14">
-      <c r="B71" s="109"/>
-      <c r="C71" s="169"/>
-      <c r="D71" s="169"/>
-      <c r="E71" s="105"/>
-      <c r="F71" s="169"/>
-      <c r="G71" s="106"/>
-      <c r="H71" s="186"/>
-      <c r="I71" s="186"/>
-      <c r="J71" s="105"/>
-      <c r="K71" s="186"/>
-      <c r="L71" s="106"/>
-      <c r="M71" s="105"/>
-    </row>
-    <row r="72" spans="2:13" ht="14">
-      <c r="B72" s="109"/>
-      <c r="C72" s="187"/>
-      <c r="D72" s="187"/>
-      <c r="E72" s="105"/>
-      <c r="F72" s="187"/>
-      <c r="G72" s="115"/>
-      <c r="H72" s="186"/>
-      <c r="I72" s="186"/>
-      <c r="J72" s="105"/>
-      <c r="K72" s="186"/>
-      <c r="L72" s="106"/>
-      <c r="M72" s="105"/>
-    </row>
-    <row r="73" spans="2:13" ht="14">
-      <c r="B73" s="109"/>
-      <c r="C73" s="189"/>
-      <c r="D73" s="189"/>
-      <c r="E73" s="105"/>
-      <c r="F73" s="189"/>
-      <c r="G73" s="115"/>
-      <c r="H73" s="186"/>
-      <c r="I73" s="186"/>
-      <c r="J73" s="105"/>
-      <c r="K73" s="186"/>
-      <c r="L73" s="106"/>
-      <c r="M73" s="105"/>
-    </row>
-    <row r="74" spans="2:13" ht="14">
-      <c r="B74" s="109"/>
-      <c r="C74" s="189"/>
-      <c r="D74" s="189"/>
-      <c r="E74" s="105"/>
-      <c r="F74" s="189"/>
-      <c r="G74" s="115"/>
-      <c r="H74" s="186"/>
-      <c r="I74" s="186"/>
-      <c r="J74" s="105"/>
-      <c r="K74" s="186"/>
-      <c r="L74" s="106"/>
-      <c r="M74" s="105"/>
-    </row>
-    <row r="75" spans="2:13" ht="14">
-      <c r="B75" s="185"/>
-      <c r="C75" s="190"/>
-      <c r="D75" s="190"/>
-      <c r="E75" s="190"/>
-      <c r="F75" s="190"/>
-      <c r="G75" s="115"/>
-      <c r="H75" s="190"/>
-      <c r="I75" s="190"/>
-      <c r="J75" s="190"/>
-      <c r="K75" s="190"/>
-      <c r="L75" s="115"/>
-      <c r="M75" s="105"/>
-    </row>
-    <row r="76" spans="2:13" ht="14">
-      <c r="B76" s="192"/>
-      <c r="C76" s="106"/>
-      <c r="D76" s="109"/>
-      <c r="E76" s="106"/>
-      <c r="F76" s="106"/>
-      <c r="G76" s="106"/>
-      <c r="H76" s="106"/>
-      <c r="I76" s="105"/>
-      <c r="J76" s="105"/>
-      <c r="K76" s="105"/>
-      <c r="L76" s="106"/>
-      <c r="M76" s="105"/>
-    </row>
-    <row r="77" spans="2:13" ht="14">
-      <c r="B77" s="191"/>
-      <c r="C77" s="106"/>
-      <c r="D77" s="106"/>
-      <c r="E77" s="105"/>
-      <c r="F77" s="106"/>
-      <c r="G77" s="106"/>
-      <c r="H77" s="106"/>
-      <c r="I77" s="106"/>
-      <c r="J77" s="105"/>
-      <c r="K77" s="106"/>
-      <c r="L77" s="106"/>
-      <c r="M77" s="126"/>
-    </row>
-    <row r="78" spans="2:13" ht="14">
-      <c r="B78" s="188"/>
-      <c r="C78" s="106"/>
-      <c r="D78" s="106"/>
-      <c r="E78" s="105"/>
-      <c r="F78" s="106"/>
-      <c r="G78" s="106"/>
-      <c r="H78" s="123"/>
-      <c r="I78" s="106"/>
-      <c r="J78" s="105"/>
-      <c r="K78" s="106"/>
-      <c r="L78" s="106"/>
-      <c r="M78" s="126"/>
-    </row>
-    <row r="79" spans="2:13" ht="14">
-      <c r="B79" s="109"/>
-      <c r="C79" s="106"/>
-      <c r="D79" s="109"/>
-      <c r="E79" s="105"/>
-      <c r="F79" s="106"/>
-      <c r="G79" s="106"/>
-      <c r="H79" s="106"/>
-      <c r="I79" s="105"/>
-      <c r="J79" s="105"/>
-      <c r="K79" s="106"/>
-      <c r="L79" s="106"/>
-      <c r="M79" s="126"/>
-    </row>
-    <row r="80" spans="2:13" ht="14">
-      <c r="B80" s="109"/>
-      <c r="C80" s="106"/>
-      <c r="D80" s="109"/>
-      <c r="E80" s="105"/>
-      <c r="F80" s="105"/>
-      <c r="G80" s="106"/>
-      <c r="H80" s="106"/>
-      <c r="I80" s="105"/>
-      <c r="J80" s="105"/>
-      <c r="K80" s="105"/>
-      <c r="L80" s="106"/>
-      <c r="M80" s="105"/>
-    </row>
-    <row r="81" spans="2:13" ht="14">
-      <c r="B81" s="193"/>
-      <c r="C81" s="106"/>
-      <c r="D81" s="106"/>
-      <c r="E81" s="106"/>
-      <c r="F81" s="106"/>
-      <c r="G81" s="106"/>
-      <c r="H81" s="106"/>
-      <c r="I81" s="106"/>
-      <c r="J81" s="105"/>
-      <c r="K81" s="106"/>
-      <c r="L81" s="106"/>
-      <c r="M81" s="126"/>
-    </row>
-    <row r="82" spans="2:13" ht="14">
-      <c r="B82" s="193"/>
-      <c r="C82" s="106"/>
-      <c r="D82" s="106"/>
-      <c r="E82" s="106"/>
-      <c r="F82" s="106"/>
-      <c r="G82" s="106"/>
-      <c r="H82" s="106"/>
-      <c r="I82" s="106"/>
-      <c r="J82" s="105"/>
-      <c r="K82" s="106"/>
-      <c r="L82" s="106"/>
-      <c r="M82" s="126"/>
-    </row>
-    <row r="83" spans="2:13" ht="14">
-      <c r="B83" s="193"/>
-      <c r="C83" s="194"/>
-      <c r="D83" s="194"/>
-      <c r="E83" s="194"/>
-      <c r="F83" s="194"/>
-      <c r="G83" s="106"/>
-      <c r="H83" s="106"/>
-      <c r="I83" s="105"/>
-      <c r="J83" s="105"/>
-      <c r="K83" s="105"/>
-      <c r="L83" s="106"/>
-      <c r="M83" s="126"/>
-    </row>
-    <row r="84" spans="2:13" ht="14">
-      <c r="B84" s="109"/>
-      <c r="C84" s="106"/>
-      <c r="D84" s="109"/>
-      <c r="E84" s="105"/>
-      <c r="F84" s="105"/>
-      <c r="G84" s="106"/>
-      <c r="H84" s="106"/>
-      <c r="I84" s="105"/>
-      <c r="J84" s="105"/>
-      <c r="K84" s="105"/>
-      <c r="L84" s="106"/>
-      <c r="M84" s="126"/>
-    </row>
-    <row r="85" spans="2:13" ht="14">
-      <c r="B85" s="109"/>
-      <c r="C85" s="106"/>
-      <c r="D85" s="109"/>
-      <c r="E85" s="105"/>
-      <c r="F85" s="105"/>
-      <c r="G85" s="106"/>
-      <c r="H85" s="106"/>
-      <c r="I85" s="105"/>
-      <c r="J85" s="105"/>
-      <c r="K85" s="105"/>
-      <c r="L85" s="106"/>
-      <c r="M85" s="105"/>
-    </row>
-    <row r="86" spans="2:13" ht="14">
-      <c r="B86" s="109"/>
-      <c r="C86" s="106"/>
-      <c r="D86" s="109"/>
-      <c r="E86" s="105"/>
-      <c r="F86" s="105"/>
-      <c r="G86" s="106"/>
-      <c r="H86" s="106"/>
-      <c r="I86" s="106"/>
-      <c r="J86" s="106"/>
-      <c r="K86" s="106"/>
-      <c r="L86" s="106"/>
-      <c r="M86" s="105"/>
-    </row>
-    <row r="87" spans="2:13" ht="14">
-      <c r="B87" s="109"/>
-      <c r="C87" s="106"/>
-      <c r="D87" s="109"/>
-      <c r="E87" s="105"/>
-      <c r="F87" s="105"/>
-      <c r="G87" s="106"/>
-      <c r="H87" s="106"/>
-      <c r="I87" s="105"/>
-      <c r="J87" s="105"/>
-      <c r="K87" s="105"/>
-      <c r="L87" s="106"/>
-      <c r="M87" s="105"/>
-    </row>
-    <row r="88" spans="2:13" ht="14">
-      <c r="B88" s="109"/>
-      <c r="C88" s="106"/>
-      <c r="D88" s="109"/>
-      <c r="E88" s="105"/>
-      <c r="F88" s="105"/>
-      <c r="G88" s="106"/>
-      <c r="H88" s="106"/>
-      <c r="I88" s="105"/>
-      <c r="J88" s="105"/>
-      <c r="K88" s="105"/>
-      <c r="L88" s="106"/>
-      <c r="M88" s="105"/>
-    </row>
-    <row r="89" spans="2:13" ht="14">
-      <c r="B89" s="109"/>
-      <c r="C89" s="106"/>
-      <c r="D89" s="109"/>
-      <c r="E89" s="105"/>
-      <c r="F89" s="105"/>
-      <c r="G89" s="106"/>
-      <c r="H89" s="106"/>
-      <c r="I89" s="105"/>
-      <c r="J89" s="105"/>
-      <c r="K89" s="105"/>
-      <c r="L89" s="106"/>
-      <c r="M89" s="105"/>
-    </row>
-    <row r="90" spans="2:13" ht="14">
-      <c r="B90" s="109"/>
-      <c r="C90" s="106"/>
-      <c r="D90" s="109"/>
-      <c r="E90" s="105"/>
-      <c r="F90" s="105"/>
-      <c r="G90" s="106"/>
-      <c r="H90" s="106"/>
-      <c r="I90" s="105"/>
-      <c r="J90" s="105"/>
-      <c r="K90" s="105"/>
-      <c r="L90" s="106"/>
-      <c r="M90" s="105"/>
-    </row>
-    <row r="91" spans="2:13" ht="14">
-      <c r="B91" s="109"/>
-      <c r="C91" s="106"/>
-      <c r="D91" s="109"/>
-      <c r="E91" s="105"/>
-      <c r="F91" s="105"/>
-      <c r="G91" s="106"/>
-      <c r="H91" s="106"/>
-      <c r="I91" s="105"/>
-      <c r="J91" s="105"/>
-      <c r="K91" s="105"/>
-      <c r="L91" s="106"/>
-      <c r="M91" s="105"/>
-    </row>
-    <row r="92" spans="2:13" ht="14">
-      <c r="B92" s="109"/>
-      <c r="C92" s="106"/>
-      <c r="D92" s="109"/>
-      <c r="E92" s="105"/>
-      <c r="F92" s="105"/>
-      <c r="G92" s="106"/>
-      <c r="H92" s="106"/>
-      <c r="I92" s="105"/>
-      <c r="J92" s="105"/>
-      <c r="K92" s="105"/>
-      <c r="L92" s="106"/>
-      <c r="M92" s="105"/>
-    </row>
-    <row r="93" spans="2:13" ht="14">
-      <c r="B93" s="109"/>
-      <c r="C93" s="106"/>
-      <c r="D93" s="109"/>
-      <c r="E93" s="105"/>
-      <c r="F93" s="105"/>
-      <c r="G93" s="106"/>
-      <c r="H93" s="106"/>
-      <c r="I93" s="105"/>
-      <c r="J93" s="105"/>
-      <c r="K93" s="105"/>
-      <c r="L93" s="106"/>
-      <c r="M93" s="105"/>
-    </row>
-    <row r="94" spans="2:13" ht="14">
-      <c r="B94" s="109"/>
-      <c r="C94" s="106"/>
-      <c r="D94" s="109"/>
-      <c r="E94" s="105"/>
-      <c r="F94" s="105"/>
-      <c r="G94" s="106"/>
-      <c r="H94" s="106"/>
-      <c r="I94" s="105"/>
-      <c r="J94" s="105"/>
-      <c r="K94" s="105"/>
-      <c r="L94" s="106"/>
-      <c r="M94" s="105"/>
-    </row>
-    <row r="95" spans="2:13" ht="14">
-      <c r="B95" s="109"/>
-      <c r="C95" s="106"/>
-      <c r="D95" s="109"/>
-      <c r="E95" s="105"/>
-      <c r="F95" s="105"/>
-      <c r="G95" s="106"/>
-      <c r="H95" s="106"/>
-      <c r="I95" s="105"/>
-      <c r="J95" s="105"/>
-      <c r="K95" s="105"/>
-      <c r="L95" s="106"/>
-      <c r="M95" s="105"/>
-    </row>
-    <row r="96" spans="2:13" ht="14">
-      <c r="B96" s="109"/>
-      <c r="C96" s="106"/>
-      <c r="D96" s="109"/>
-      <c r="E96" s="105"/>
-      <c r="F96" s="105"/>
-      <c r="G96" s="106"/>
-      <c r="H96" s="106"/>
-      <c r="I96" s="105"/>
-      <c r="J96" s="105"/>
-      <c r="K96" s="105"/>
-      <c r="L96" s="106"/>
-      <c r="M96" s="105"/>
-    </row>
-    <row r="97" spans="2:13" ht="14">
-      <c r="B97" s="109"/>
-      <c r="C97" s="106"/>
-      <c r="D97" s="109"/>
-      <c r="E97" s="105"/>
-      <c r="F97" s="105"/>
-      <c r="G97" s="106"/>
-      <c r="H97" s="106"/>
-      <c r="I97" s="105"/>
-      <c r="J97" s="105"/>
-      <c r="K97" s="105"/>
-      <c r="L97" s="106"/>
-      <c r="M97" s="105"/>
-    </row>
-    <row r="98" spans="2:13" ht="14">
-      <c r="B98" s="109"/>
-      <c r="C98" s="106"/>
-      <c r="D98" s="109"/>
-      <c r="E98" s="105"/>
-      <c r="F98" s="105"/>
-      <c r="G98" s="106"/>
-      <c r="H98" s="106"/>
-      <c r="I98" s="105"/>
-      <c r="J98" s="105"/>
-      <c r="K98" s="105"/>
-      <c r="L98" s="106"/>
-      <c r="M98" s="105"/>
-    </row>
-    <row r="99" spans="2:13" ht="14">
-      <c r="B99" s="109"/>
-      <c r="C99" s="106"/>
-      <c r="D99" s="109"/>
-      <c r="E99" s="105"/>
-      <c r="F99" s="105"/>
-      <c r="G99" s="106"/>
-      <c r="H99" s="106"/>
-      <c r="I99" s="105"/>
-      <c r="J99" s="105"/>
-      <c r="K99" s="105"/>
-      <c r="L99" s="106"/>
-      <c r="M99" s="105"/>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>